<commit_message>
Updated Attachment E Mod 5
Updated Attachment E Mod 5 based on meeting
</commit_message>
<xml_diff>
--- a/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -69,60 +69,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>nayan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Section 9</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>nayan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Section 4.4</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -250,71 +202,77 @@
     <t>q</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/PM/ADS%20Project%20Plan.doc</t>
+    <t>evidence #1</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/PM/MOM/MOM06172015.docx</t>
+    <t>evidence #2</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Functional%20Spec/MOM%20-%20UX%20Design%2006182015.docx</t>
+    <t xml:space="preserve">              </t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Functional%20Spec/MOM%20-%20UX%20Design%2006192015.docx</t>
+    <t>ADS Project Plan. Section 6.2: Project Organization Chart</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/Interaction%20withUXTeam.docx</t>
+    <t>Project Initiation Meeting Minutes</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Engg/Src/UI/app/styles/bootstrap-theme.css</t>
+    <t>Meeting with End User Group on 18 June 2015</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/issues/20</t>
+    <t>Meeting with End User Group on 19 June 2015</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/issues/22</t>
+    <t>User Centric Design Techniques</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/UI%20on%20Android.jpg</t>
+    <t>Twitter Bootstrap Style Cheet from the Codebase</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/UI%20on%20Iphone.jpg</t>
+    <t>Issues reported by User Group</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Engg/Design/Documents/dAnalytics-Design%20document%20.docx</t>
+    <t>Screenshot of dAnalytics on Android Phone</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/aws_instances.png</t>
+    <t>Screenshot of dAnalytics on Apple iPhone</t>
   </si>
   <si>
-    <t>http://danalytics.tpgsi.com</t>
+    <t>dAnalytics Design Document - Section 9 : Technology Stack</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Engg/Src/REST/openfda-service/src/test/java/context/TestContext.java</t>
+    <t>Screenshot of deployment on Amazon Web Services</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/QA/TestPlan_danalytics.doc</t>
+    <t>JUnit Test Case</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/Travis%20ScreenShot.jpg</t>
+    <t>dAnalytics Test Plan</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics</t>
+    <t>Screenshot of Travis for Continous Integration</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Engg/Design/Documents/dAnalytics-Installation%20document.docx</t>
+    <t>URL for GitHub Repository</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/Monit%20Screenshot.JPG</t>
+    <t>Screenshot of Monit for Continous Monitoring</t>
   </si>
   <si>
-    <t>https://github.com/TPRockville/dAnalytics/blob/master/Req/Storyboard/MonitEmailScreenshot.JPG</t>
+    <t>Email From Monit for Process Status</t>
+  </si>
+  <si>
+    <t>dAnalytics Deployment Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dAnalytics design Document. Section </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -361,26 +319,19 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -411,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -431,6 +382,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11001,8 +10955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11023,9 +10977,11 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
@@ -11037,10 +10993,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -11053,7 +11009,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="2"/>
@@ -11067,10 +11023,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -11083,7 +11039,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="2"/>
@@ -11097,7 +11053,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
@@ -11111,10 +11067,10 @@
         <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -11127,10 +11083,10 @@
         <v>23</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -11143,10 +11099,10 @@
         <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -11159,7 +11115,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
@@ -11173,11 +11129,9 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>54</v>
-      </c>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
@@ -11189,10 +11143,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -11205,7 +11159,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="2"/>
@@ -11219,11 +11173,9 @@
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="5" t="s">
         <v>59</v>
       </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
@@ -11250,7 +11202,7 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -11263,7 +11215,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="2"/>
@@ -11276,7 +11228,9 @@
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -11311,7 +11265,9 @@
     <row r="24" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="25" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -16191,21 +16147,25 @@
     <hyperlink ref="C5" r:id="rId4"/>
     <hyperlink ref="C4" r:id="rId5"/>
     <hyperlink ref="D4" r:id="rId6"/>
-    <hyperlink ref="D8" r:id="rId7"/>
-    <hyperlink ref="C8" r:id="rId8"/>
-    <hyperlink ref="C10" r:id="rId9"/>
-    <hyperlink ref="C15" r:id="rId10"/>
-    <hyperlink ref="D15" r:id="rId11"/>
-    <hyperlink ref="C17" r:id="rId12"/>
-    <hyperlink ref="C6" r:id="rId13"/>
-    <hyperlink ref="D2" r:id="rId14"/>
-    <hyperlink ref="C9" r:id="rId15"/>
+    <hyperlink ref="C10" r:id="rId7"/>
+    <hyperlink ref="C15" r:id="rId8"/>
+    <hyperlink ref="D15" r:id="rId9"/>
+    <hyperlink ref="C6" r:id="rId10"/>
+    <hyperlink ref="D2" r:id="rId11"/>
+    <hyperlink ref="C9" r:id="rId12"/>
+    <hyperlink ref="C3" r:id="rId13"/>
+    <hyperlink ref="D12" r:id="rId14"/>
+    <hyperlink ref="D9" r:id="rId15"/>
     <hyperlink ref="C2" r:id="rId16"/>
-    <hyperlink ref="C3" r:id="rId17"/>
-    <hyperlink ref="D12" r:id="rId18"/>
-    <hyperlink ref="D9" r:id="rId19"/>
+    <hyperlink ref="C7" r:id="rId17"/>
+    <hyperlink ref="D7" r:id="rId18"/>
+    <hyperlink ref="C8" r:id="rId19"/>
+    <hyperlink ref="D8" r:id="rId20"/>
+    <hyperlink ref="C11" r:id="rId21"/>
+    <hyperlink ref="C17" r:id="rId22"/>
+    <hyperlink ref="C18" r:id="rId23"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId20"/>
+  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attachment E updated with Docker Screenshot
Attachment E updated with Docker Screenshot
</commit_message>
<xml_diff>
--- a/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -15,66 +15,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>nayan</author>
-  </authors>
-  <commentList>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>nayan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Section 6.2</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>nayan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Section 6.2</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
   <si>
     <t>#</t>
   </si>
@@ -223,13 +165,7 @@
     <t>Meeting with End User Group on 19 June 2015</t>
   </si>
   <si>
-    <t>User Centric Design Techniques</t>
-  </si>
-  <si>
     <t>Twitter Bootstrap Style Cheet from the Codebase</t>
-  </si>
-  <si>
-    <t>Issues reported by User Group</t>
   </si>
   <si>
     <t>Screenshot of dAnalytics on Android Phone</t>
@@ -265,14 +201,26 @@
     <t>dAnalytics Deployment Document</t>
   </si>
   <si>
-    <t xml:space="preserve">dAnalytics design Document. Section </t>
+    <t>dAnalytics design Document. Section 9.11 Licenses for the third party platforms/tools used</t>
+  </si>
+  <si>
+    <t>Human Centric Design Techniques</t>
+  </si>
+  <si>
+    <t>Issues reported by User Group - Github ticket</t>
+  </si>
+  <si>
+    <t>Issues reported by User Group - Github Ticket</t>
+  </si>
+  <si>
+    <t>Screenshot of Docker - Deployment Container for DAnalytics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -306,32 +254,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -362,7 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -382,9 +311,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10952,11 +10878,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11039,7 +10965,7 @@
         <v>27</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="2"/>
@@ -11053,7 +10979,7 @@
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="2"/>
@@ -11067,10 +10993,10 @@
         <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -11099,10 +11025,10 @@
         <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -11115,7 +11041,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="2"/>
@@ -11129,7 +11055,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -11143,10 +11069,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -11159,7 +11085,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="2"/>
@@ -11173,7 +11099,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -11187,10 +11113,10 @@
         <v>18</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -11202,7 +11128,9 @@
       <c r="B16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="7" t="s">
+        <v>65</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -11215,7 +11143,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="2"/>
@@ -11228,8 +11156,8 @@
       <c r="B18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>63</v>
+      <c r="C18" s="7" t="s">
+        <v>61</v>
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="2"/>
@@ -16164,8 +16092,8 @@
     <hyperlink ref="C11" r:id="rId21"/>
     <hyperlink ref="C17" r:id="rId22"/>
     <hyperlink ref="C18" r:id="rId23"/>
+    <hyperlink ref="C16" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Attachment E Updated. Minor Edits.
</commit_message>
<xml_diff>
--- a/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
+++ b/PM/Attachment E Approach Criteria Evidence Template Mod 5.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="70">
   <si>
     <t>#</t>
   </si>
@@ -215,6 +215,18 @@
   <si>
     <t>Screenshot of Docker - Deployment Container for DAnalytics</t>
   </si>
+  <si>
+    <t>Meeting with End User Group (Real People) on 19 June 2015</t>
+  </si>
+  <si>
+    <t>Meeting with End User Group (Real People) on 18 June 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Cases and Performance Test results </t>
+  </si>
+  <si>
+    <t>evidence #3</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -311,6 +323,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10882,7 +10897,7 @@
   <dimension ref="A1:F998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -10890,8 +10905,9 @@
     <col min="1" max="1" width="9.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="59.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="54.28515625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" style="3" customWidth="1"/>
-    <col min="5" max="26" width="14.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="3" customWidth="1"/>
+    <col min="6" max="26" width="14.42578125" style="3" customWidth="1"/>
     <col min="27" max="16384" width="17.28515625" style="3"/>
   </cols>
   <sheetData>
@@ -10908,7 +10924,9 @@
       <c r="D1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -10949,10 +10967,10 @@
         <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -11074,7 +11092,9 @@
       <c r="D12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
@@ -16093,6 +16113,7 @@
     <hyperlink ref="C17" r:id="rId22"/>
     <hyperlink ref="C18" r:id="rId23"/>
     <hyperlink ref="C16" r:id="rId24"/>
+    <hyperlink ref="E12" r:id="rId25"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>